<commit_message>
- Info actualizada y correccion de direcciones
</commit_message>
<xml_diff>
--- a/nuevosScripts/diccionarios/diccionarios.xlsx
+++ b/nuevosScripts/diccionarios/diccionarios.xlsx
@@ -5,18 +5,19 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Mis proyectos\Test\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Mis proyectos\Test\Repo-Python-DB-DottAPI\nuevosScripts\diccionarios\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C08E621D-AFDA-4AFE-95F5-7E7F7AAA0960}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E447531-5836-4CD1-81A3-B429733B3699}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{907ADB49-8BB7-4046-9511-7212E4DA76A7}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{907ADB49-8BB7-4046-9511-7212E4DA76A7}"/>
   </bookViews>
   <sheets>
     <sheet name="Air" sheetId="1" r:id="rId1"/>
     <sheet name="Eik" sheetId="2" r:id="rId2"/>
     <sheet name="Elit" sheetId="3" r:id="rId3"/>
     <sheet name="NB" sheetId="4" r:id="rId4"/>
+    <sheet name="Categorias" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2671" uniqueCount="357">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2704" uniqueCount="377">
   <si>
     <t>electro</t>
   </si>
@@ -1099,6 +1100,66 @@
   </si>
   <si>
     <t>NOTEBOOKS - CLOUDBOOKS</t>
+  </si>
+  <si>
+    <t>Categoria</t>
+  </si>
+  <si>
+    <t>Cables y Adaptadores</t>
+  </si>
+  <si>
+    <t>Computadoras</t>
+  </si>
+  <si>
+    <t>Conectividad</t>
+  </si>
+  <si>
+    <t>Discos</t>
+  </si>
+  <si>
+    <t>Electro</t>
+  </si>
+  <si>
+    <t>Estabilizadores y UPS</t>
+  </si>
+  <si>
+    <t>Gamer</t>
+  </si>
+  <si>
+    <t>Impresoras e Insumos</t>
+  </si>
+  <si>
+    <t>Memorias RAM</t>
+  </si>
+  <si>
+    <t>Almacenamiento Portatil</t>
+  </si>
+  <si>
+    <t>Notebooks</t>
+  </si>
+  <si>
+    <t>Placas de video</t>
+  </si>
+  <si>
+    <t>Proyectores</t>
+  </si>
+  <si>
+    <t>Refrigeracion</t>
+  </si>
+  <si>
+    <t>Smartwatch</t>
+  </si>
+  <si>
+    <t>Software</t>
+  </si>
+  <si>
+    <t>Tablets</t>
+  </si>
+  <si>
+    <t>Telefonia</t>
+  </si>
+  <si>
+    <t>Webcams</t>
   </si>
 </sst>
 </file>
@@ -10419,7 +10480,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C9A83B5-C2A8-42F3-A50B-B65DA1F9C1BC}">
   <dimension ref="A1:I45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+    <sheetView topLeftCell="A8" workbookViewId="0">
       <selection activeCell="K25" sqref="K25"/>
     </sheetView>
   </sheetViews>
@@ -11783,4 +11844,185 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29A23AC8-0680-4338-8F9B-085C30FD02CA}">
+  <dimension ref="A1:A33"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:A33"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1">
+      <c r="A5" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1">
+      <c r="A6" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1">
+      <c r="A7" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1">
+      <c r="A8" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1">
+      <c r="A9" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1">
+      <c r="A10" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1">
+      <c r="A11" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1">
+      <c r="A12" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1">
+      <c r="A13" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1">
+      <c r="A14" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1">
+      <c r="A15" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1">
+      <c r="A16" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1">
+      <c r="A17" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1">
+      <c r="A18" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1">
+      <c r="A19" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1">
+      <c r="A20" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1">
+      <c r="A21" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1">
+      <c r="A22" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1">
+      <c r="A23" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1">
+      <c r="A24" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1">
+      <c r="A25" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1">
+      <c r="A26" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1">
+      <c r="A27" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1">
+      <c r="A28" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1">
+      <c r="A29" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1">
+      <c r="A30" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1">
+      <c r="A31" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1">
+      <c r="A32" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1">
+      <c r="A33" t="s">
+        <v>376</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
- Se agregan mas cositas
</commit_message>
<xml_diff>
--- a/nuevosScripts/diccionarios/diccionarios.xlsx
+++ b/nuevosScripts/diccionarios/diccionarios.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Mis proyectos\Test\Repo-Python-DB-DottAPI\nuevosScripts\diccionarios\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BAD95A8-CEDB-4E01-9EF8-B661CD780DE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB16F52B-46BD-4D73-9661-18E3349F910E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{907ADB49-8BB7-4046-9511-7212E4DA76A7}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17205" windowHeight="15600" activeTab="5" xr2:uid="{907ADB49-8BB7-4046-9511-7212E4DA76A7}"/>
   </bookViews>
   <sheets>
     <sheet name="Air" sheetId="1" r:id="rId1"/>
@@ -18,8 +18,9 @@
     <sheet name="Elit" sheetId="3" r:id="rId3"/>
     <sheet name="Invid" sheetId="6" r:id="rId4"/>
     <sheet name="Megacom" sheetId="7" r:id="rId5"/>
-    <sheet name="NB" sheetId="4" r:id="rId6"/>
-    <sheet name="Categorias" sheetId="5" r:id="rId7"/>
+    <sheet name="Hdc" sheetId="8" r:id="rId6"/>
+    <sheet name="NB" sheetId="4" r:id="rId7"/>
+    <sheet name="Categorias" sheetId="5" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4465" uniqueCount="577">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4977" uniqueCount="630">
   <si>
     <t>electro</t>
   </si>
@@ -1762,6 +1763,165 @@
   </si>
   <si>
     <t>Discos Rígidos / SSD / Disco Rígido Notebook</t>
+  </si>
+  <si>
+    <t>10"</t>
+  </si>
+  <si>
+    <t>12"</t>
+  </si>
+  <si>
+    <t>2 Canales</t>
+  </si>
+  <si>
+    <t>4"</t>
+  </si>
+  <si>
+    <t>6.5"</t>
+  </si>
+  <si>
+    <t>6x9"</t>
+  </si>
+  <si>
+    <t>8"</t>
+  </si>
+  <si>
+    <t>Accesorios Gaming</t>
+  </si>
+  <si>
+    <t>Amplificador</t>
+  </si>
+  <si>
+    <t>Audio Home</t>
+  </si>
+  <si>
+    <t>Barbijos</t>
+  </si>
+  <si>
+    <t>Barras de Sonido</t>
+  </si>
+  <si>
+    <t>Baterías</t>
+  </si>
+  <si>
+    <t>Camaras de Seguridad</t>
+  </si>
+  <si>
+    <t>Cascos</t>
+  </si>
+  <si>
+    <t>Combo</t>
+  </si>
+  <si>
+    <t>Cooler</t>
+  </si>
+  <si>
+    <t>Din</t>
+  </si>
+  <si>
+    <t>Din-Doble</t>
+  </si>
+  <si>
+    <t>Disco Rigido Interno</t>
+  </si>
+  <si>
+    <t>DVR</t>
+  </si>
+  <si>
+    <t>Earbud</t>
+  </si>
+  <si>
+    <t>Ebook</t>
+  </si>
+  <si>
+    <t>Fuente de Poder</t>
+  </si>
+  <si>
+    <t>Gabinete Sin Fuente</t>
+  </si>
+  <si>
+    <t>Gabinetes KIT</t>
+  </si>
+  <si>
+    <t>Hogar</t>
+  </si>
+  <si>
+    <t>In Ear</t>
+  </si>
+  <si>
+    <t>Kit Teclado Y Mouse</t>
+  </si>
+  <si>
+    <t>Memoria Notebooks</t>
+  </si>
+  <si>
+    <t>Microfono</t>
+  </si>
+  <si>
+    <t>Microprocesador Intel</t>
+  </si>
+  <si>
+    <t>Monoblock</t>
+  </si>
+  <si>
+    <t>Notebook</t>
+  </si>
+  <si>
+    <t>On Ear</t>
+  </si>
+  <si>
+    <t>Pad Mouse</t>
+  </si>
+  <si>
+    <t>Parlante Bluetooth</t>
+  </si>
+  <si>
+    <t>Parlante Portátil</t>
+  </si>
+  <si>
+    <t>Parlantes Pc</t>
+  </si>
+  <si>
+    <t>Party Speaker</t>
+  </si>
+  <si>
+    <t>Pc De Escritorio</t>
+  </si>
+  <si>
+    <t>Productos</t>
+  </si>
+  <si>
+    <t>Salud</t>
+  </si>
+  <si>
+    <t>SSD</t>
+  </si>
+  <si>
+    <t>SSD Externo</t>
+  </si>
+  <si>
+    <t>Stereo</t>
+  </si>
+  <si>
+    <t>Subwoofer</t>
+  </si>
+  <si>
+    <t>Tablet</t>
+  </si>
+  <si>
+    <t>Torre de Sonido</t>
+  </si>
+  <si>
+    <t>TV</t>
+  </si>
+  <si>
+    <t>Varios</t>
+  </si>
+  <si>
+    <t>WEBCAM</t>
+  </si>
+  <si>
+    <t>Monitoress</t>
   </si>
 </sst>
 </file>
@@ -13465,7 +13625,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CDC37D85-05AB-4705-A6FD-F8425FE0B657}">
   <dimension ref="A1:I141"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
@@ -17713,6 +17873,1947 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2BA0658-C126-4173-B7A6-ED504D386D93}">
+  <dimension ref="A1:I64"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="H36" sqref="H36"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="39" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9">
+      <c r="A1" t="s">
+        <v>178</v>
+      </c>
+      <c r="B1" t="s">
+        <v>577</v>
+      </c>
+      <c r="C1" t="s">
+        <v>178</v>
+      </c>
+      <c r="D1" t="s">
+        <v>263</v>
+      </c>
+      <c r="E1" t="s">
+        <v>178</v>
+      </c>
+      <c r="F1" t="s">
+        <v>298</v>
+      </c>
+      <c r="G1" t="s">
+        <v>178</v>
+      </c>
+      <c r="H1" t="s">
+        <v>179</v>
+      </c>
+      <c r="I1" t="str">
+        <f>_xlfn.CONCAT(A1:H1)</f>
+        <v>"10"":"Parlantes",</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
+      <c r="A2" t="s">
+        <v>178</v>
+      </c>
+      <c r="B2" t="s">
+        <v>578</v>
+      </c>
+      <c r="C2" t="s">
+        <v>178</v>
+      </c>
+      <c r="D2" t="s">
+        <v>263</v>
+      </c>
+      <c r="E2" t="s">
+        <v>178</v>
+      </c>
+      <c r="F2" t="s">
+        <v>298</v>
+      </c>
+      <c r="G2" t="s">
+        <v>178</v>
+      </c>
+      <c r="H2" t="s">
+        <v>179</v>
+      </c>
+      <c r="I2" t="str">
+        <f t="shared" ref="I2:I64" si="0">_xlfn.CONCAT(A2:H2)</f>
+        <v>"12"":"Parlantes",</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="A3" t="s">
+        <v>178</v>
+      </c>
+      <c r="B3" t="s">
+        <v>579</v>
+      </c>
+      <c r="C3" t="s">
+        <v>178</v>
+      </c>
+      <c r="D3" t="s">
+        <v>263</v>
+      </c>
+      <c r="E3" t="s">
+        <v>178</v>
+      </c>
+      <c r="F3" t="s">
+        <v>298</v>
+      </c>
+      <c r="G3" t="s">
+        <v>178</v>
+      </c>
+      <c r="H3" t="s">
+        <v>179</v>
+      </c>
+      <c r="I3" t="str">
+        <f t="shared" si="0"/>
+        <v>"2 Canales":"Parlantes",</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="A4" t="s">
+        <v>178</v>
+      </c>
+      <c r="B4" t="s">
+        <v>580</v>
+      </c>
+      <c r="C4" t="s">
+        <v>178</v>
+      </c>
+      <c r="D4" t="s">
+        <v>263</v>
+      </c>
+      <c r="E4" t="s">
+        <v>178</v>
+      </c>
+      <c r="F4" t="s">
+        <v>298</v>
+      </c>
+      <c r="G4" t="s">
+        <v>178</v>
+      </c>
+      <c r="H4" t="s">
+        <v>179</v>
+      </c>
+      <c r="I4" t="str">
+        <f t="shared" si="0"/>
+        <v>"4"":"Parlantes",</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="A5" t="s">
+        <v>178</v>
+      </c>
+      <c r="B5" t="s">
+        <v>581</v>
+      </c>
+      <c r="C5" t="s">
+        <v>178</v>
+      </c>
+      <c r="D5" t="s">
+        <v>263</v>
+      </c>
+      <c r="E5" t="s">
+        <v>178</v>
+      </c>
+      <c r="F5" t="s">
+        <v>298</v>
+      </c>
+      <c r="G5" t="s">
+        <v>178</v>
+      </c>
+      <c r="H5" t="s">
+        <v>179</v>
+      </c>
+      <c r="I5" t="str">
+        <f t="shared" si="0"/>
+        <v>"6.5"":"Parlantes",</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="A6" t="s">
+        <v>178</v>
+      </c>
+      <c r="B6" t="s">
+        <v>582</v>
+      </c>
+      <c r="C6" t="s">
+        <v>178</v>
+      </c>
+      <c r="D6" t="s">
+        <v>263</v>
+      </c>
+      <c r="E6" t="s">
+        <v>178</v>
+      </c>
+      <c r="F6" t="s">
+        <v>298</v>
+      </c>
+      <c r="G6" t="s">
+        <v>178</v>
+      </c>
+      <c r="H6" t="s">
+        <v>179</v>
+      </c>
+      <c r="I6" t="str">
+        <f t="shared" si="0"/>
+        <v>"6x9"":"Parlantes",</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="A7" t="s">
+        <v>178</v>
+      </c>
+      <c r="B7" t="s">
+        <v>583</v>
+      </c>
+      <c r="C7" t="s">
+        <v>178</v>
+      </c>
+      <c r="D7" t="s">
+        <v>263</v>
+      </c>
+      <c r="E7" t="s">
+        <v>178</v>
+      </c>
+      <c r="F7" t="s">
+        <v>298</v>
+      </c>
+      <c r="G7" t="s">
+        <v>178</v>
+      </c>
+      <c r="H7" t="s">
+        <v>179</v>
+      </c>
+      <c r="I7" t="str">
+        <f t="shared" si="0"/>
+        <v>"8"":"Parlantes",</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="A8" t="s">
+        <v>178</v>
+      </c>
+      <c r="B8" t="s">
+        <v>264</v>
+      </c>
+      <c r="C8" t="s">
+        <v>178</v>
+      </c>
+      <c r="D8" t="s">
+        <v>263</v>
+      </c>
+      <c r="E8" t="s">
+        <v>178</v>
+      </c>
+      <c r="F8" t="s">
+        <v>264</v>
+      </c>
+      <c r="G8" t="s">
+        <v>178</v>
+      </c>
+      <c r="H8" t="s">
+        <v>179</v>
+      </c>
+      <c r="I8" t="str">
+        <f t="shared" si="0"/>
+        <v>"Accesorios":"Accesorios",</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="A9" t="s">
+        <v>178</v>
+      </c>
+      <c r="B9" t="s">
+        <v>584</v>
+      </c>
+      <c r="C9" t="s">
+        <v>178</v>
+      </c>
+      <c r="D9" t="s">
+        <v>263</v>
+      </c>
+      <c r="E9" t="s">
+        <v>178</v>
+      </c>
+      <c r="F9" t="s">
+        <v>264</v>
+      </c>
+      <c r="G9" t="s">
+        <v>178</v>
+      </c>
+      <c r="H9" t="s">
+        <v>179</v>
+      </c>
+      <c r="I9" t="str">
+        <f t="shared" si="0"/>
+        <v>"Accesorios Gaming":"Accesorios",</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="A10" t="s">
+        <v>178</v>
+      </c>
+      <c r="B10" t="s">
+        <v>585</v>
+      </c>
+      <c r="C10" t="s">
+        <v>178</v>
+      </c>
+      <c r="D10" t="s">
+        <v>263</v>
+      </c>
+      <c r="E10" t="s">
+        <v>178</v>
+      </c>
+      <c r="F10" t="s">
+        <v>298</v>
+      </c>
+      <c r="G10" t="s">
+        <v>178</v>
+      </c>
+      <c r="H10" t="s">
+        <v>179</v>
+      </c>
+      <c r="I10" t="str">
+        <f t="shared" si="0"/>
+        <v>"Amplificador":"Parlantes",</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
+      <c r="A11" t="s">
+        <v>178</v>
+      </c>
+      <c r="B11" t="s">
+        <v>586</v>
+      </c>
+      <c r="C11" t="s">
+        <v>178</v>
+      </c>
+      <c r="D11" t="s">
+        <v>263</v>
+      </c>
+      <c r="E11" t="s">
+        <v>178</v>
+      </c>
+      <c r="F11" t="s">
+        <v>362</v>
+      </c>
+      <c r="G11" t="s">
+        <v>178</v>
+      </c>
+      <c r="H11" t="s">
+        <v>179</v>
+      </c>
+      <c r="I11" t="str">
+        <f t="shared" si="0"/>
+        <v>"Audio Home":"Electro",</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
+      <c r="A12" t="s">
+        <v>178</v>
+      </c>
+      <c r="B12" t="s">
+        <v>267</v>
+      </c>
+      <c r="C12" t="s">
+        <v>178</v>
+      </c>
+      <c r="D12" t="s">
+        <v>263</v>
+      </c>
+      <c r="E12" t="s">
+        <v>178</v>
+      </c>
+      <c r="F12" t="s">
+        <v>267</v>
+      </c>
+      <c r="G12" t="s">
+        <v>178</v>
+      </c>
+      <c r="H12" t="s">
+        <v>179</v>
+      </c>
+      <c r="I12" t="str">
+        <f t="shared" si="0"/>
+        <v>"Auriculares":"Auriculares",</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9">
+      <c r="A13" t="s">
+        <v>178</v>
+      </c>
+      <c r="B13" t="s">
+        <v>587</v>
+      </c>
+      <c r="C13" t="s">
+        <v>178</v>
+      </c>
+      <c r="D13" t="s">
+        <v>263</v>
+      </c>
+      <c r="E13" t="s">
+        <v>178</v>
+      </c>
+      <c r="F13" t="s">
+        <v>264</v>
+      </c>
+      <c r="G13" t="s">
+        <v>178</v>
+      </c>
+      <c r="H13" t="s">
+        <v>179</v>
+      </c>
+      <c r="I13" t="str">
+        <f t="shared" si="0"/>
+        <v>"Barbijos":"Accesorios",</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9">
+      <c r="A14" t="s">
+        <v>178</v>
+      </c>
+      <c r="B14" t="s">
+        <v>588</v>
+      </c>
+      <c r="C14" t="s">
+        <v>178</v>
+      </c>
+      <c r="D14" t="s">
+        <v>263</v>
+      </c>
+      <c r="E14" t="s">
+        <v>178</v>
+      </c>
+      <c r="F14" t="s">
+        <v>298</v>
+      </c>
+      <c r="G14" t="s">
+        <v>178</v>
+      </c>
+      <c r="H14" t="s">
+        <v>179</v>
+      </c>
+      <c r="I14" t="str">
+        <f t="shared" si="0"/>
+        <v>"Barras de Sonido":"Parlantes",</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9">
+      <c r="A15" t="s">
+        <v>178</v>
+      </c>
+      <c r="B15" t="s">
+        <v>589</v>
+      </c>
+      <c r="C15" t="s">
+        <v>178</v>
+      </c>
+      <c r="D15" t="s">
+        <v>263</v>
+      </c>
+      <c r="E15" t="s">
+        <v>178</v>
+      </c>
+      <c r="F15" t="s">
+        <v>264</v>
+      </c>
+      <c r="G15" t="s">
+        <v>178</v>
+      </c>
+      <c r="H15" t="s">
+        <v>179</v>
+      </c>
+      <c r="I15" t="str">
+        <f t="shared" si="0"/>
+        <v>"Baterías":"Accesorios",</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9">
+      <c r="A16" t="s">
+        <v>178</v>
+      </c>
+      <c r="B16" t="s">
+        <v>590</v>
+      </c>
+      <c r="C16" t="s">
+        <v>178</v>
+      </c>
+      <c r="D16" t="s">
+        <v>263</v>
+      </c>
+      <c r="E16" t="s">
+        <v>178</v>
+      </c>
+      <c r="F16" t="s">
+        <v>360</v>
+      </c>
+      <c r="G16" t="s">
+        <v>178</v>
+      </c>
+      <c r="H16" t="s">
+        <v>179</v>
+      </c>
+      <c r="I16" t="str">
+        <f t="shared" si="0"/>
+        <v>"Camaras de Seguridad":"Conectividad",</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9">
+      <c r="A17" t="s">
+        <v>178</v>
+      </c>
+      <c r="B17" t="s">
+        <v>591</v>
+      </c>
+      <c r="C17" t="s">
+        <v>178</v>
+      </c>
+      <c r="D17" t="s">
+        <v>263</v>
+      </c>
+      <c r="E17" t="s">
+        <v>178</v>
+      </c>
+      <c r="F17" t="s">
+        <v>362</v>
+      </c>
+      <c r="G17" t="s">
+        <v>178</v>
+      </c>
+      <c r="H17" t="s">
+        <v>179</v>
+      </c>
+      <c r="I17" t="str">
+        <f t="shared" si="0"/>
+        <v>"Cascos":"Electro",</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9">
+      <c r="A18" t="s">
+        <v>178</v>
+      </c>
+      <c r="B18" t="s">
+        <v>478</v>
+      </c>
+      <c r="C18" t="s">
+        <v>178</v>
+      </c>
+      <c r="D18" t="s">
+        <v>263</v>
+      </c>
+      <c r="E18" t="s">
+        <v>178</v>
+      </c>
+      <c r="F18" t="s">
+        <v>375</v>
+      </c>
+      <c r="G18" t="s">
+        <v>178</v>
+      </c>
+      <c r="H18" t="s">
+        <v>179</v>
+      </c>
+      <c r="I18" t="str">
+        <f t="shared" si="0"/>
+        <v>"Celulares":"Telefonia",</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9">
+      <c r="A19" t="s">
+        <v>178</v>
+      </c>
+      <c r="B19" t="s">
+        <v>592</v>
+      </c>
+      <c r="C19" t="s">
+        <v>178</v>
+      </c>
+      <c r="D19" t="s">
+        <v>263</v>
+      </c>
+      <c r="E19" t="s">
+        <v>178</v>
+      </c>
+      <c r="F19" t="s">
+        <v>364</v>
+      </c>
+      <c r="G19" t="s">
+        <v>178</v>
+      </c>
+      <c r="H19" t="s">
+        <v>179</v>
+      </c>
+      <c r="I19" t="str">
+        <f t="shared" si="0"/>
+        <v>"Combo":"Gamer",</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9">
+      <c r="A20" t="s">
+        <v>178</v>
+      </c>
+      <c r="B20" t="s">
+        <v>593</v>
+      </c>
+      <c r="C20" t="s">
+        <v>178</v>
+      </c>
+      <c r="D20" t="s">
+        <v>263</v>
+      </c>
+      <c r="E20" t="s">
+        <v>178</v>
+      </c>
+      <c r="F20" t="s">
+        <v>371</v>
+      </c>
+      <c r="G20" t="s">
+        <v>178</v>
+      </c>
+      <c r="H20" t="s">
+        <v>179</v>
+      </c>
+      <c r="I20" t="str">
+        <f t="shared" si="0"/>
+        <v>"Cooler":"Refrigeracion",</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9">
+      <c r="A21" t="s">
+        <v>178</v>
+      </c>
+      <c r="B21" t="s">
+        <v>594</v>
+      </c>
+      <c r="C21" t="s">
+        <v>178</v>
+      </c>
+      <c r="D21" t="s">
+        <v>263</v>
+      </c>
+      <c r="E21" t="s">
+        <v>178</v>
+      </c>
+      <c r="F21" t="s">
+        <v>362</v>
+      </c>
+      <c r="G21" t="s">
+        <v>178</v>
+      </c>
+      <c r="H21" t="s">
+        <v>179</v>
+      </c>
+      <c r="I21" t="str">
+        <f t="shared" si="0"/>
+        <v>"Din":"Electro",</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9">
+      <c r="A22" t="s">
+        <v>178</v>
+      </c>
+      <c r="B22" t="s">
+        <v>595</v>
+      </c>
+      <c r="C22" t="s">
+        <v>178</v>
+      </c>
+      <c r="D22" t="s">
+        <v>263</v>
+      </c>
+      <c r="E22" t="s">
+        <v>178</v>
+      </c>
+      <c r="F22" t="s">
+        <v>362</v>
+      </c>
+      <c r="G22" t="s">
+        <v>178</v>
+      </c>
+      <c r="H22" t="s">
+        <v>179</v>
+      </c>
+      <c r="I22" t="str">
+        <f t="shared" si="0"/>
+        <v>"Din-Doble":"Electro",</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9">
+      <c r="A23" t="s">
+        <v>178</v>
+      </c>
+      <c r="B23" t="s">
+        <v>596</v>
+      </c>
+      <c r="C23" t="s">
+        <v>178</v>
+      </c>
+      <c r="D23" t="s">
+        <v>263</v>
+      </c>
+      <c r="E23" t="s">
+        <v>178</v>
+      </c>
+      <c r="F23" t="s">
+        <v>361</v>
+      </c>
+      <c r="G23" t="s">
+        <v>178</v>
+      </c>
+      <c r="H23" t="s">
+        <v>179</v>
+      </c>
+      <c r="I23" t="str">
+        <f t="shared" si="0"/>
+        <v>"Disco Rigido Interno":"Discos",</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9">
+      <c r="A24" t="s">
+        <v>178</v>
+      </c>
+      <c r="B24" t="s">
+        <v>597</v>
+      </c>
+      <c r="C24" t="s">
+        <v>178</v>
+      </c>
+      <c r="D24" t="s">
+        <v>263</v>
+      </c>
+      <c r="E24" t="s">
+        <v>178</v>
+      </c>
+      <c r="F24" t="s">
+        <v>360</v>
+      </c>
+      <c r="G24" t="s">
+        <v>178</v>
+      </c>
+      <c r="H24" t="s">
+        <v>179</v>
+      </c>
+      <c r="I24" t="str">
+        <f t="shared" si="0"/>
+        <v>"DVR":"Conectividad",</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9">
+      <c r="A25" t="s">
+        <v>178</v>
+      </c>
+      <c r="B25" t="s">
+        <v>598</v>
+      </c>
+      <c r="C25" t="s">
+        <v>178</v>
+      </c>
+      <c r="D25" t="s">
+        <v>263</v>
+      </c>
+      <c r="E25" t="s">
+        <v>178</v>
+      </c>
+      <c r="F25" t="s">
+        <v>267</v>
+      </c>
+      <c r="G25" t="s">
+        <v>178</v>
+      </c>
+      <c r="H25" t="s">
+        <v>179</v>
+      </c>
+      <c r="I25" t="str">
+        <f t="shared" si="0"/>
+        <v>"Earbud":"Auriculares",</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9">
+      <c r="A26" t="s">
+        <v>178</v>
+      </c>
+      <c r="B26" t="s">
+        <v>599</v>
+      </c>
+      <c r="C26" t="s">
+        <v>178</v>
+      </c>
+      <c r="D26" t="s">
+        <v>263</v>
+      </c>
+      <c r="E26" t="s">
+        <v>178</v>
+      </c>
+      <c r="F26" t="s">
+        <v>362</v>
+      </c>
+      <c r="G26" t="s">
+        <v>178</v>
+      </c>
+      <c r="H26" t="s">
+        <v>179</v>
+      </c>
+      <c r="I26" t="str">
+        <f t="shared" si="0"/>
+        <v>"Ebook":"Electro",</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9">
+      <c r="A27" t="s">
+        <v>178</v>
+      </c>
+      <c r="B27" t="s">
+        <v>600</v>
+      </c>
+      <c r="C27" t="s">
+        <v>178</v>
+      </c>
+      <c r="D27" t="s">
+        <v>263</v>
+      </c>
+      <c r="E27" t="s">
+        <v>178</v>
+      </c>
+      <c r="F27" t="s">
+        <v>283</v>
+      </c>
+      <c r="G27" t="s">
+        <v>178</v>
+      </c>
+      <c r="H27" t="s">
+        <v>179</v>
+      </c>
+      <c r="I27" t="str">
+        <f t="shared" si="0"/>
+        <v>"Fuente de Poder":"Fuentes",</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9">
+      <c r="A28" t="s">
+        <v>178</v>
+      </c>
+      <c r="B28" t="s">
+        <v>601</v>
+      </c>
+      <c r="C28" t="s">
+        <v>178</v>
+      </c>
+      <c r="D28" t="s">
+        <v>263</v>
+      </c>
+      <c r="E28" t="s">
+        <v>178</v>
+      </c>
+      <c r="F28" t="s">
+        <v>285</v>
+      </c>
+      <c r="G28" t="s">
+        <v>178</v>
+      </c>
+      <c r="H28" t="s">
+        <v>179</v>
+      </c>
+      <c r="I28" t="str">
+        <f t="shared" si="0"/>
+        <v>"Gabinete Sin Fuente":"Gabinetes",</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9">
+      <c r="A29" t="s">
+        <v>178</v>
+      </c>
+      <c r="B29" t="s">
+        <v>602</v>
+      </c>
+      <c r="C29" t="s">
+        <v>178</v>
+      </c>
+      <c r="D29" t="s">
+        <v>263</v>
+      </c>
+      <c r="E29" t="s">
+        <v>178</v>
+      </c>
+      <c r="F29" t="s">
+        <v>285</v>
+      </c>
+      <c r="G29" t="s">
+        <v>178</v>
+      </c>
+      <c r="H29" t="s">
+        <v>179</v>
+      </c>
+      <c r="I29" t="str">
+        <f t="shared" si="0"/>
+        <v>"Gabinetes KIT":"Gabinetes",</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9">
+      <c r="A30" t="s">
+        <v>178</v>
+      </c>
+      <c r="B30" t="s">
+        <v>603</v>
+      </c>
+      <c r="C30" t="s">
+        <v>178</v>
+      </c>
+      <c r="D30" t="s">
+        <v>263</v>
+      </c>
+      <c r="E30" t="s">
+        <v>178</v>
+      </c>
+      <c r="F30" t="s">
+        <v>362</v>
+      </c>
+      <c r="G30" t="s">
+        <v>178</v>
+      </c>
+      <c r="H30" t="s">
+        <v>179</v>
+      </c>
+      <c r="I30" t="str">
+        <f t="shared" si="0"/>
+        <v>"Hogar":"Electro",</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9">
+      <c r="A31" t="s">
+        <v>178</v>
+      </c>
+      <c r="B31" t="s">
+        <v>604</v>
+      </c>
+      <c r="C31" t="s">
+        <v>178</v>
+      </c>
+      <c r="D31" t="s">
+        <v>263</v>
+      </c>
+      <c r="E31" t="s">
+        <v>178</v>
+      </c>
+      <c r="F31" t="s">
+        <v>267</v>
+      </c>
+      <c r="G31" t="s">
+        <v>178</v>
+      </c>
+      <c r="H31" t="s">
+        <v>179</v>
+      </c>
+      <c r="I31" t="str">
+        <f t="shared" si="0"/>
+        <v>"In Ear":"Auriculares",</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9">
+      <c r="A32" t="s">
+        <v>178</v>
+      </c>
+      <c r="B32" t="s">
+        <v>605</v>
+      </c>
+      <c r="C32" t="s">
+        <v>178</v>
+      </c>
+      <c r="D32" t="s">
+        <v>263</v>
+      </c>
+      <c r="E32" t="s">
+        <v>178</v>
+      </c>
+      <c r="F32" t="s">
+        <v>311</v>
+      </c>
+      <c r="G32" t="s">
+        <v>178</v>
+      </c>
+      <c r="H32" t="s">
+        <v>179</v>
+      </c>
+      <c r="I32" t="str">
+        <f t="shared" si="0"/>
+        <v>"Kit Teclado Y Mouse":"Teclados",</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9">
+      <c r="A33" t="s">
+        <v>178</v>
+      </c>
+      <c r="B33" t="s">
+        <v>606</v>
+      </c>
+      <c r="C33" t="s">
+        <v>178</v>
+      </c>
+      <c r="D33" t="s">
+        <v>263</v>
+      </c>
+      <c r="E33" t="s">
+        <v>178</v>
+      </c>
+      <c r="F33" t="s">
+        <v>366</v>
+      </c>
+      <c r="G33" t="s">
+        <v>178</v>
+      </c>
+      <c r="H33" t="s">
+        <v>179</v>
+      </c>
+      <c r="I33" t="str">
+        <f t="shared" si="0"/>
+        <v>"Memoria Notebooks":"Memorias RAM",</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9">
+      <c r="A34" t="s">
+        <v>178</v>
+      </c>
+      <c r="B34" t="s">
+        <v>291</v>
+      </c>
+      <c r="C34" t="s">
+        <v>178</v>
+      </c>
+      <c r="D34" t="s">
+        <v>263</v>
+      </c>
+      <c r="E34" t="s">
+        <v>178</v>
+      </c>
+      <c r="F34" t="s">
+        <v>366</v>
+      </c>
+      <c r="G34" t="s">
+        <v>178</v>
+      </c>
+      <c r="H34" t="s">
+        <v>179</v>
+      </c>
+      <c r="I34" t="str">
+        <f t="shared" si="0"/>
+        <v>"Memorias PC":"Memorias RAM",</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9">
+      <c r="A35" t="s">
+        <v>178</v>
+      </c>
+      <c r="B35" t="s">
+        <v>607</v>
+      </c>
+      <c r="C35" t="s">
+        <v>178</v>
+      </c>
+      <c r="D35" t="s">
+        <v>263</v>
+      </c>
+      <c r="E35" t="s">
+        <v>178</v>
+      </c>
+      <c r="F35" t="s">
+        <v>292</v>
+      </c>
+      <c r="G35" t="s">
+        <v>178</v>
+      </c>
+      <c r="H35" t="s">
+        <v>179</v>
+      </c>
+      <c r="I35" t="str">
+        <f t="shared" si="0"/>
+        <v>"Microfono":"Microfonos",</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9">
+      <c r="A36" t="s">
+        <v>178</v>
+      </c>
+      <c r="B36" t="s">
+        <v>608</v>
+      </c>
+      <c r="C36" t="s">
+        <v>178</v>
+      </c>
+      <c r="D36" t="s">
+        <v>263</v>
+      </c>
+      <c r="E36" t="s">
+        <v>178</v>
+      </c>
+      <c r="F36" t="s">
+        <v>302</v>
+      </c>
+      <c r="G36" t="s">
+        <v>178</v>
+      </c>
+      <c r="H36" t="s">
+        <v>179</v>
+      </c>
+      <c r="I36" t="str">
+        <f t="shared" si="0"/>
+        <v>"Microprocesador Intel":"Procesadores",</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9">
+      <c r="A37" t="s">
+        <v>178</v>
+      </c>
+      <c r="B37" t="s">
+        <v>293</v>
+      </c>
+      <c r="C37" t="s">
+        <v>178</v>
+      </c>
+      <c r="D37" t="s">
+        <v>263</v>
+      </c>
+      <c r="E37" t="s">
+        <v>178</v>
+      </c>
+      <c r="F37" t="s">
+        <v>629</v>
+      </c>
+      <c r="G37" t="s">
+        <v>178</v>
+      </c>
+      <c r="H37" t="s">
+        <v>179</v>
+      </c>
+      <c r="I37" t="str">
+        <f t="shared" si="0"/>
+        <v>"Monitores":"Monitoress",</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9">
+      <c r="A38" t="s">
+        <v>178</v>
+      </c>
+      <c r="B38" t="s">
+        <v>609</v>
+      </c>
+      <c r="C38" t="s">
+        <v>178</v>
+      </c>
+      <c r="D38" t="s">
+        <v>263</v>
+      </c>
+      <c r="E38" t="s">
+        <v>178</v>
+      </c>
+      <c r="F38" t="s">
+        <v>362</v>
+      </c>
+      <c r="G38" t="s">
+        <v>178</v>
+      </c>
+      <c r="H38" t="s">
+        <v>179</v>
+      </c>
+      <c r="I38" t="str">
+        <f t="shared" si="0"/>
+        <v>"Monoblock":"Electro",</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9">
+      <c r="A39" t="s">
+        <v>178</v>
+      </c>
+      <c r="B39" t="s">
+        <v>295</v>
+      </c>
+      <c r="C39" t="s">
+        <v>178</v>
+      </c>
+      <c r="D39" t="s">
+        <v>263</v>
+      </c>
+      <c r="E39" t="s">
+        <v>178</v>
+      </c>
+      <c r="F39" t="s">
+        <v>295</v>
+      </c>
+      <c r="G39" t="s">
+        <v>178</v>
+      </c>
+      <c r="H39" t="s">
+        <v>179</v>
+      </c>
+      <c r="I39" t="str">
+        <f t="shared" si="0"/>
+        <v>"Mouses":"Mouses",</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9">
+      <c r="A40" t="s">
+        <v>178</v>
+      </c>
+      <c r="B40" t="s">
+        <v>610</v>
+      </c>
+      <c r="C40" t="s">
+        <v>178</v>
+      </c>
+      <c r="D40" t="s">
+        <v>263</v>
+      </c>
+      <c r="E40" t="s">
+        <v>178</v>
+      </c>
+      <c r="F40" t="s">
+        <v>368</v>
+      </c>
+      <c r="G40" t="s">
+        <v>178</v>
+      </c>
+      <c r="H40" t="s">
+        <v>179</v>
+      </c>
+      <c r="I40" t="str">
+        <f t="shared" si="0"/>
+        <v>"Notebook":"Notebooks",</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9">
+      <c r="A41" t="s">
+        <v>178</v>
+      </c>
+      <c r="B41" t="s">
+        <v>611</v>
+      </c>
+      <c r="C41" t="s">
+        <v>178</v>
+      </c>
+      <c r="D41" t="s">
+        <v>263</v>
+      </c>
+      <c r="E41" t="s">
+        <v>178</v>
+      </c>
+      <c r="F41" t="s">
+        <v>267</v>
+      </c>
+      <c r="G41" t="s">
+        <v>178</v>
+      </c>
+      <c r="H41" t="s">
+        <v>179</v>
+      </c>
+      <c r="I41" t="str">
+        <f t="shared" si="0"/>
+        <v>"On Ear":"Auriculares",</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9">
+      <c r="A42" t="s">
+        <v>178</v>
+      </c>
+      <c r="B42" t="s">
+        <v>612</v>
+      </c>
+      <c r="C42" t="s">
+        <v>178</v>
+      </c>
+      <c r="D42" t="s">
+        <v>263</v>
+      </c>
+      <c r="E42" t="s">
+        <v>178</v>
+      </c>
+      <c r="F42" t="s">
+        <v>295</v>
+      </c>
+      <c r="G42" t="s">
+        <v>178</v>
+      </c>
+      <c r="H42" t="s">
+        <v>179</v>
+      </c>
+      <c r="I42" t="str">
+        <f t="shared" si="0"/>
+        <v>"Pad Mouse":"Mouses",</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9">
+      <c r="A43" t="s">
+        <v>178</v>
+      </c>
+      <c r="B43" t="s">
+        <v>613</v>
+      </c>
+      <c r="C43" t="s">
+        <v>178</v>
+      </c>
+      <c r="D43" t="s">
+        <v>263</v>
+      </c>
+      <c r="E43" t="s">
+        <v>178</v>
+      </c>
+      <c r="F43" t="s">
+        <v>298</v>
+      </c>
+      <c r="G43" t="s">
+        <v>178</v>
+      </c>
+      <c r="H43" t="s">
+        <v>179</v>
+      </c>
+      <c r="I43" t="str">
+        <f t="shared" si="0"/>
+        <v>"Parlante Bluetooth":"Parlantes",</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9">
+      <c r="A44" t="s">
+        <v>178</v>
+      </c>
+      <c r="B44" t="s">
+        <v>614</v>
+      </c>
+      <c r="C44" t="s">
+        <v>178</v>
+      </c>
+      <c r="D44" t="s">
+        <v>263</v>
+      </c>
+      <c r="E44" t="s">
+        <v>178</v>
+      </c>
+      <c r="F44" t="s">
+        <v>298</v>
+      </c>
+      <c r="G44" t="s">
+        <v>178</v>
+      </c>
+      <c r="H44" t="s">
+        <v>179</v>
+      </c>
+      <c r="I44" t="str">
+        <f t="shared" si="0"/>
+        <v>"Parlante Portátil":"Parlantes",</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9">
+      <c r="A45" t="s">
+        <v>178</v>
+      </c>
+      <c r="B45" t="s">
+        <v>298</v>
+      </c>
+      <c r="C45" t="s">
+        <v>178</v>
+      </c>
+      <c r="D45" t="s">
+        <v>263</v>
+      </c>
+      <c r="E45" t="s">
+        <v>178</v>
+      </c>
+      <c r="F45" t="s">
+        <v>298</v>
+      </c>
+      <c r="G45" t="s">
+        <v>178</v>
+      </c>
+      <c r="H45" t="s">
+        <v>179</v>
+      </c>
+      <c r="I45" t="str">
+        <f t="shared" si="0"/>
+        <v>"Parlantes":"Parlantes",</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9">
+      <c r="A46" t="s">
+        <v>178</v>
+      </c>
+      <c r="B46" t="s">
+        <v>615</v>
+      </c>
+      <c r="C46" t="s">
+        <v>178</v>
+      </c>
+      <c r="D46" t="s">
+        <v>263</v>
+      </c>
+      <c r="E46" t="s">
+        <v>178</v>
+      </c>
+      <c r="F46" t="s">
+        <v>298</v>
+      </c>
+      <c r="G46" t="s">
+        <v>178</v>
+      </c>
+      <c r="H46" t="s">
+        <v>179</v>
+      </c>
+      <c r="I46" t="str">
+        <f t="shared" si="0"/>
+        <v>"Parlantes Pc":"Parlantes",</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9">
+      <c r="A47" t="s">
+        <v>178</v>
+      </c>
+      <c r="B47" t="s">
+        <v>616</v>
+      </c>
+      <c r="C47" t="s">
+        <v>178</v>
+      </c>
+      <c r="D47" t="s">
+        <v>263</v>
+      </c>
+      <c r="E47" t="s">
+        <v>178</v>
+      </c>
+      <c r="F47" t="s">
+        <v>298</v>
+      </c>
+      <c r="G47" t="s">
+        <v>178</v>
+      </c>
+      <c r="H47" t="s">
+        <v>179</v>
+      </c>
+      <c r="I47" t="str">
+        <f t="shared" si="0"/>
+        <v>"Party Speaker":"Parlantes",</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9">
+      <c r="A48" t="s">
+        <v>178</v>
+      </c>
+      <c r="B48" t="s">
+        <v>617</v>
+      </c>
+      <c r="C48" t="s">
+        <v>178</v>
+      </c>
+      <c r="D48" t="s">
+        <v>263</v>
+      </c>
+      <c r="E48" t="s">
+        <v>178</v>
+      </c>
+      <c r="F48" t="s">
+        <v>359</v>
+      </c>
+      <c r="G48" t="s">
+        <v>178</v>
+      </c>
+      <c r="H48" t="s">
+        <v>179</v>
+      </c>
+      <c r="I48" t="str">
+        <f t="shared" si="0"/>
+        <v>"Pc De Escritorio":"Computadoras",</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9">
+      <c r="A49" t="s">
+        <v>178</v>
+      </c>
+      <c r="B49" t="s">
+        <v>318</v>
+      </c>
+      <c r="C49" t="s">
+        <v>178</v>
+      </c>
+      <c r="D49" t="s">
+        <v>263</v>
+      </c>
+      <c r="E49" t="s">
+        <v>178</v>
+      </c>
+      <c r="F49" t="s">
+        <v>369</v>
+      </c>
+      <c r="G49" t="s">
+        <v>178</v>
+      </c>
+      <c r="H49" t="s">
+        <v>179</v>
+      </c>
+      <c r="I49" t="str">
+        <f t="shared" si="0"/>
+        <v>"Placas de Video":"Placas de video",</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9">
+      <c r="A50" t="s">
+        <v>178</v>
+      </c>
+      <c r="B50" t="s">
+        <v>618</v>
+      </c>
+      <c r="C50" t="s">
+        <v>178</v>
+      </c>
+      <c r="D50" t="s">
+        <v>263</v>
+      </c>
+      <c r="E50" t="s">
+        <v>178</v>
+      </c>
+      <c r="F50" t="s">
+        <v>374</v>
+      </c>
+      <c r="G50" t="s">
+        <v>178</v>
+      </c>
+      <c r="H50" t="s">
+        <v>179</v>
+      </c>
+      <c r="I50" t="str">
+        <f t="shared" si="0"/>
+        <v>"Productos":"Tablets",</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9">
+      <c r="A51" t="s">
+        <v>178</v>
+      </c>
+      <c r="B51" t="s">
+        <v>550</v>
+      </c>
+      <c r="C51" t="s">
+        <v>178</v>
+      </c>
+      <c r="D51" t="s">
+        <v>263</v>
+      </c>
+      <c r="E51" t="s">
+        <v>178</v>
+      </c>
+      <c r="F51" t="s">
+        <v>362</v>
+      </c>
+      <c r="G51" t="s">
+        <v>178</v>
+      </c>
+      <c r="H51" t="s">
+        <v>179</v>
+      </c>
+      <c r="I51" t="str">
+        <f t="shared" si="0"/>
+        <v>"Repuestos":"Electro",</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9">
+      <c r="A52" t="s">
+        <v>178</v>
+      </c>
+      <c r="B52" t="s">
+        <v>305</v>
+      </c>
+      <c r="C52" t="s">
+        <v>178</v>
+      </c>
+      <c r="D52" t="s">
+        <v>263</v>
+      </c>
+      <c r="E52" t="s">
+        <v>178</v>
+      </c>
+      <c r="F52" t="s">
+        <v>360</v>
+      </c>
+      <c r="G52" t="s">
+        <v>178</v>
+      </c>
+      <c r="H52" t="s">
+        <v>179</v>
+      </c>
+      <c r="I52" t="str">
+        <f t="shared" si="0"/>
+        <v>"Routers":"Conectividad",</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9">
+      <c r="A53" t="s">
+        <v>178</v>
+      </c>
+      <c r="B53" t="s">
+        <v>619</v>
+      </c>
+      <c r="C53" t="s">
+        <v>178</v>
+      </c>
+      <c r="D53" t="s">
+        <v>263</v>
+      </c>
+      <c r="E53" t="s">
+        <v>178</v>
+      </c>
+      <c r="F53" t="s">
+        <v>362</v>
+      </c>
+      <c r="G53" t="s">
+        <v>178</v>
+      </c>
+      <c r="H53" t="s">
+        <v>179</v>
+      </c>
+      <c r="I53" t="str">
+        <f t="shared" si="0"/>
+        <v>"Salud":"Electro",</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9">
+      <c r="A54" t="s">
+        <v>178</v>
+      </c>
+      <c r="B54" t="s">
+        <v>306</v>
+      </c>
+      <c r="C54" t="s">
+        <v>178</v>
+      </c>
+      <c r="D54" t="s">
+        <v>263</v>
+      </c>
+      <c r="E54" t="s">
+        <v>178</v>
+      </c>
+      <c r="F54" t="s">
+        <v>306</v>
+      </c>
+      <c r="G54" t="s">
+        <v>178</v>
+      </c>
+      <c r="H54" t="s">
+        <v>179</v>
+      </c>
+      <c r="I54" t="str">
+        <f t="shared" si="0"/>
+        <v>"Sillas":"Sillas",</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9">
+      <c r="A55" t="s">
+        <v>178</v>
+      </c>
+      <c r="B55" t="s">
+        <v>620</v>
+      </c>
+      <c r="C55" t="s">
+        <v>178</v>
+      </c>
+      <c r="D55" t="s">
+        <v>263</v>
+      </c>
+      <c r="E55" t="s">
+        <v>178</v>
+      </c>
+      <c r="F55" t="s">
+        <v>361</v>
+      </c>
+      <c r="G55" t="s">
+        <v>178</v>
+      </c>
+      <c r="H55" t="s">
+        <v>179</v>
+      </c>
+      <c r="I55" t="str">
+        <f t="shared" si="0"/>
+        <v>"SSD":"Discos",</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9">
+      <c r="A56" t="s">
+        <v>178</v>
+      </c>
+      <c r="B56" t="s">
+        <v>621</v>
+      </c>
+      <c r="C56" t="s">
+        <v>178</v>
+      </c>
+      <c r="D56" t="s">
+        <v>263</v>
+      </c>
+      <c r="E56" t="s">
+        <v>178</v>
+      </c>
+      <c r="F56" t="s">
+        <v>367</v>
+      </c>
+      <c r="G56" t="s">
+        <v>178</v>
+      </c>
+      <c r="H56" t="s">
+        <v>179</v>
+      </c>
+      <c r="I56" t="str">
+        <f t="shared" si="0"/>
+        <v>"SSD Externo":"Almacenamiento Portatil",</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9">
+      <c r="A57" t="s">
+        <v>178</v>
+      </c>
+      <c r="B57" t="s">
+        <v>622</v>
+      </c>
+      <c r="C57" t="s">
+        <v>178</v>
+      </c>
+      <c r="D57" t="s">
+        <v>263</v>
+      </c>
+      <c r="E57" t="s">
+        <v>178</v>
+      </c>
+      <c r="F57" t="s">
+        <v>362</v>
+      </c>
+      <c r="G57" t="s">
+        <v>178</v>
+      </c>
+      <c r="H57" t="s">
+        <v>179</v>
+      </c>
+      <c r="I57" t="str">
+        <f t="shared" si="0"/>
+        <v>"Stereo":"Electro",</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9">
+      <c r="A58" t="s">
+        <v>178</v>
+      </c>
+      <c r="B58" t="s">
+        <v>623</v>
+      </c>
+      <c r="C58" t="s">
+        <v>178</v>
+      </c>
+      <c r="D58" t="s">
+        <v>263</v>
+      </c>
+      <c r="E58" t="s">
+        <v>178</v>
+      </c>
+      <c r="F58" t="s">
+        <v>298</v>
+      </c>
+      <c r="G58" t="s">
+        <v>178</v>
+      </c>
+      <c r="H58" t="s">
+        <v>179</v>
+      </c>
+      <c r="I58" t="str">
+        <f t="shared" si="0"/>
+        <v>"Subwoofer":"Parlantes",</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9">
+      <c r="A59" t="s">
+        <v>178</v>
+      </c>
+      <c r="B59" t="s">
+        <v>624</v>
+      </c>
+      <c r="C59" t="s">
+        <v>178</v>
+      </c>
+      <c r="D59" t="s">
+        <v>263</v>
+      </c>
+      <c r="E59" t="s">
+        <v>178</v>
+      </c>
+      <c r="F59" t="s">
+        <v>374</v>
+      </c>
+      <c r="G59" t="s">
+        <v>178</v>
+      </c>
+      <c r="H59" t="s">
+        <v>179</v>
+      </c>
+      <c r="I59" t="str">
+        <f t="shared" si="0"/>
+        <v>"Tablet":"Tablets",</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9">
+      <c r="A60" t="s">
+        <v>178</v>
+      </c>
+      <c r="B60" t="s">
+        <v>311</v>
+      </c>
+      <c r="C60" t="s">
+        <v>178</v>
+      </c>
+      <c r="D60" t="s">
+        <v>263</v>
+      </c>
+      <c r="E60" t="s">
+        <v>178</v>
+      </c>
+      <c r="F60" t="s">
+        <v>311</v>
+      </c>
+      <c r="G60" t="s">
+        <v>178</v>
+      </c>
+      <c r="H60" t="s">
+        <v>179</v>
+      </c>
+      <c r="I60" t="str">
+        <f t="shared" si="0"/>
+        <v>"Teclados":"Teclados",</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9">
+      <c r="A61" t="s">
+        <v>178</v>
+      </c>
+      <c r="B61" t="s">
+        <v>625</v>
+      </c>
+      <c r="C61" t="s">
+        <v>178</v>
+      </c>
+      <c r="D61" t="s">
+        <v>263</v>
+      </c>
+      <c r="E61" t="s">
+        <v>178</v>
+      </c>
+      <c r="F61" t="s">
+        <v>298</v>
+      </c>
+      <c r="G61" t="s">
+        <v>178</v>
+      </c>
+      <c r="H61" t="s">
+        <v>179</v>
+      </c>
+      <c r="I61" t="str">
+        <f t="shared" si="0"/>
+        <v>"Torre de Sonido":"Parlantes",</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9">
+      <c r="A62" t="s">
+        <v>178</v>
+      </c>
+      <c r="B62" t="s">
+        <v>626</v>
+      </c>
+      <c r="C62" t="s">
+        <v>178</v>
+      </c>
+      <c r="D62" t="s">
+        <v>263</v>
+      </c>
+      <c r="E62" t="s">
+        <v>178</v>
+      </c>
+      <c r="F62" t="s">
+        <v>362</v>
+      </c>
+      <c r="G62" t="s">
+        <v>178</v>
+      </c>
+      <c r="H62" t="s">
+        <v>179</v>
+      </c>
+      <c r="I62" t="str">
+        <f t="shared" si="0"/>
+        <v>"TV":"Electro",</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9">
+      <c r="A63" t="s">
+        <v>178</v>
+      </c>
+      <c r="B63" t="s">
+        <v>627</v>
+      </c>
+      <c r="C63" t="s">
+        <v>178</v>
+      </c>
+      <c r="D63" t="s">
+        <v>263</v>
+      </c>
+      <c r="E63" t="s">
+        <v>178</v>
+      </c>
+      <c r="F63" t="s">
+        <v>358</v>
+      </c>
+      <c r="G63" t="s">
+        <v>178</v>
+      </c>
+      <c r="H63" t="s">
+        <v>179</v>
+      </c>
+      <c r="I63" t="str">
+        <f t="shared" si="0"/>
+        <v>"Varios":"Cables y Adaptadores",</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9">
+      <c r="A64" t="s">
+        <v>178</v>
+      </c>
+      <c r="B64" t="s">
+        <v>628</v>
+      </c>
+      <c r="C64" t="s">
+        <v>178</v>
+      </c>
+      <c r="D64" t="s">
+        <v>263</v>
+      </c>
+      <c r="E64" t="s">
+        <v>178</v>
+      </c>
+      <c r="F64" t="s">
+        <v>376</v>
+      </c>
+      <c r="G64" t="s">
+        <v>178</v>
+      </c>
+      <c r="H64" t="s">
+        <v>179</v>
+      </c>
+      <c r="I64" t="str">
+        <f t="shared" si="0"/>
+        <v>"WEBCAM":"Webcams",</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C9A83B5-C2A8-42F3-A50B-B65DA1F9C1BC}">
   <dimension ref="A1:I45"/>
   <sheetViews>
@@ -19082,7 +21183,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29A23AC8-0680-4338-8F9B-085C30FD02CA}">
   <dimension ref="A1:A33"/>
   <sheetViews>

</xml_diff>